<commit_message>
creacion final de excels
</commit_message>
<xml_diff>
--- a/excels/organica.xlsx
+++ b/excels/organica.xlsx
@@ -451,17 +451,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4497</t>
+          <t>5478</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9037</t>
+          <t>3725</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4497-9037</t>
+          <t>5478-3725</t>
         </is>
       </c>
     </row>
@@ -473,17 +473,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3160</t>
+          <t>9803</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2078</t>
+          <t>5439</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3160-2078</t>
+          <t>9803-5439</t>
         </is>
       </c>
     </row>
@@ -495,17 +495,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4354</t>
+          <t>9494</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>9295</t>
+          <t>5942</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4354-9295</t>
+          <t>9494-5942</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4951</t>
+          <t>3662</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5307</t>
+          <t>7821</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>4951-5307</t>
+          <t>3662-7821</t>
         </is>
       </c>
     </row>
@@ -539,17 +539,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>6260</t>
+          <t>7664</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2400</t>
+          <t>6117</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6260-2400</t>
+          <t>7664-6117</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1628</t>
+          <t>1025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4074</t>
+          <t>4573</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1628-4074</t>
+          <t>1025-4573</t>
         </is>
       </c>
     </row>
@@ -583,17 +583,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1880</t>
+          <t>9554</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>662</t>
+          <t>6223</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1880-662</t>
+          <t>9554-6223</t>
         </is>
       </c>
     </row>
@@ -605,17 +605,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>3545</t>
+          <t>4942</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>4733</t>
+          <t>6392</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3545-4733</t>
+          <t>4942-6392</t>
         </is>
       </c>
     </row>
@@ -627,17 +627,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2289</t>
+          <t>4129</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1415</t>
+          <t>231</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2289-1415</t>
+          <t>4129-231</t>
         </is>
       </c>
     </row>
@@ -649,17 +649,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3745</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3811</t>
+          <t>104</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3745-3811</t>
+          <t>5682-104</t>
         </is>
       </c>
     </row>
@@ -671,17 +671,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1806</t>
+          <t>9966</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3491</t>
+          <t>9038</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1806-3491</t>
+          <t>9966-9038</t>
         </is>
       </c>
     </row>
@@ -693,17 +693,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5176</t>
+          <t>1065</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1758</t>
+          <t>7508</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>5176-1758</t>
+          <t>1065-7508</t>
         </is>
       </c>
     </row>
@@ -715,17 +715,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8404</t>
+          <t>1577</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>3932</t>
+          <t>851</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>8404-3932</t>
+          <t>1577-851</t>
         </is>
       </c>
     </row>
@@ -737,17 +737,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1950</t>
+          <t>8852</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7780</t>
+          <t>2227</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1950-7780</t>
+          <t>8852-2227</t>
         </is>
       </c>
     </row>
@@ -759,17 +759,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>9985</t>
+          <t>4488</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6267</t>
+          <t>2903</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>9985-6267</t>
+          <t>4488-2903</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>9989</t>
+          <t>1920</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>4083</t>
+          <t>4206</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>9989-4083</t>
+          <t>1920-4206</t>
         </is>
       </c>
     </row>
@@ -803,17 +803,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7693</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>8115</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>7693-182</t>
+          <t>5124-8115</t>
         </is>
       </c>
     </row>
@@ -825,17 +825,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7795</t>
+          <t>4176</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6177</t>
+          <t>5490</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>7795-6177</t>
+          <t>4176-5490</t>
         </is>
       </c>
     </row>
@@ -847,17 +847,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>9782</t>
+          <t>5962</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4301</t>
+          <t>6222</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>9782-4301</t>
+          <t>5962-6222</t>
         </is>
       </c>
     </row>
@@ -869,17 +869,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>6979</t>
+          <t>8063</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>269</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6979-389</t>
+          <t>8063-269</t>
         </is>
       </c>
     </row>
@@ -891,17 +891,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>6639</t>
+          <t>1288</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>3578</t>
+          <t>954</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6639-3578</t>
+          <t>1288-954</t>
         </is>
       </c>
     </row>
@@ -913,17 +913,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1140</t>
+          <t>8391</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>7119</t>
+          <t>237</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1140-7119</t>
+          <t>8391-237</t>
         </is>
       </c>
     </row>
@@ -935,17 +935,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>5844</t>
+          <t>6891</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>5969</t>
+          <t>3956</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5844-5969</t>
+          <t>6891-3956</t>
         </is>
       </c>
     </row>
@@ -957,17 +957,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1160</t>
+          <t>8532</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>731</t>
+          <t>8574</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1160-731</t>
+          <t>8532-8574</t>
         </is>
       </c>
     </row>
@@ -979,17 +979,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3650</t>
+          <t>8677</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>7850</t>
+          <t>6796</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3650-7850</t>
+          <t>8677-6796</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
agregar hojas a catalogo
</commit_message>
<xml_diff>
--- a/excels/organica.xlsx
+++ b/excels/organica.xlsx
@@ -451,17 +451,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>9075</t>
+          <t>4901</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6767</t>
+          <t>6432</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9075-6767</t>
+          <t>4901-6432</t>
         </is>
       </c>
     </row>
@@ -473,17 +473,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3627</t>
+          <t>6285</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8869</t>
+          <t>2107</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3627-8869</t>
+          <t>6285-2107</t>
         </is>
       </c>
     </row>
@@ -495,17 +495,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9899</t>
+          <t>8826</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4470</t>
+          <t>5895</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9899-4470</t>
+          <t>8826-5895</t>
         </is>
       </c>
     </row>
@@ -517,17 +517,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5771</t>
+          <t>3661</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4601</t>
+          <t>140</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5771-4601</t>
+          <t>3661-140</t>
         </is>
       </c>
     </row>
@@ -539,17 +539,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2676</t>
+          <t>1559</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5253</t>
+          <t>1757</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2676-5253</t>
+          <t>1559-1757</t>
         </is>
       </c>
     </row>
@@ -561,17 +561,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>7223</t>
+          <t>1416</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2506</t>
+          <t>9312</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7223-2506</t>
+          <t>1416-9312</t>
         </is>
       </c>
     </row>
@@ -583,17 +583,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7484</t>
+          <t>5554</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2401</t>
+          <t>4505</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>7484-2401</t>
+          <t>5554-4505</t>
         </is>
       </c>
     </row>
@@ -605,17 +605,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7378</t>
+          <t>8001</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>9638</t>
+          <t>2420</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7378-9638</t>
+          <t>8001-2420</t>
         </is>
       </c>
     </row>
@@ -627,17 +627,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4507</t>
+          <t>2890</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>2203</t>
+          <t>3661</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4507-2203</t>
+          <t>2890-3661</t>
         </is>
       </c>
     </row>
@@ -649,17 +649,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>3521</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5933</t>
+          <t>7427</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6182-5933</t>
+          <t>3521-7427</t>
         </is>
       </c>
     </row>
@@ -671,17 +671,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6688</t>
+          <t>3107</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>9002</t>
+          <t>2281</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6688-9002</t>
+          <t>3107-2281</t>
         </is>
       </c>
     </row>
@@ -693,17 +693,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4656</t>
+          <t>4259</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>9862</t>
+          <t>9597</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>4656-9862</t>
+          <t>4259-9597</t>
         </is>
       </c>
     </row>
@@ -715,17 +715,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1135</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5221</t>
+          <t>900</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1135-5221</t>
+          <t>6998-900</t>
         </is>
       </c>
     </row>
@@ -737,17 +737,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6862</t>
+          <t>4946</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>746</t>
+          <t>5127</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6862-746</t>
+          <t>4946-5127</t>
         </is>
       </c>
     </row>
@@ -759,17 +759,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1414</t>
+          <t>1909</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>4545</t>
+          <t>7235</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1414-4545</t>
+          <t>1909-7235</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3347</t>
+          <t>8551</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>614</t>
+          <t>1639</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3347-614</t>
+          <t>8551-1639</t>
         </is>
       </c>
     </row>
@@ -803,17 +803,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5407</t>
+          <t>4694</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>647</t>
+          <t>438</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5407-647</t>
+          <t>4694-438</t>
         </is>
       </c>
     </row>
@@ -825,17 +825,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7835</t>
+          <t>2578</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>947</t>
+          <t>6562</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>7835-947</t>
+          <t>2578-6562</t>
         </is>
       </c>
     </row>
@@ -847,17 +847,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>6992</t>
+          <t>8435</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5446</t>
+          <t>1694</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6992-5446</t>
+          <t>8435-1694</t>
         </is>
       </c>
     </row>
@@ -869,17 +869,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4705</t>
+          <t>6858</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4603</t>
+          <t>2659</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>4705-4603</t>
+          <t>6858-2659</t>
         </is>
       </c>
     </row>
@@ -891,17 +891,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3128</t>
+          <t>2964</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5600</t>
+          <t>2268</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3128-5600</t>
+          <t>2964-2268</t>
         </is>
       </c>
     </row>
@@ -913,17 +913,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1368</t>
+          <t>3236</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>583</t>
+          <t>2170</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>1368-583</t>
+          <t>3236-2170</t>
         </is>
       </c>
     </row>
@@ -935,17 +935,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7966</t>
+          <t>1465</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2694</t>
+          <t>1783</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>7966-2694</t>
+          <t>1465-1783</t>
         </is>
       </c>
     </row>
@@ -957,17 +957,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>7649</t>
+          <t>7462</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>8130</t>
+          <t>4192</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>7649-8130</t>
+          <t>7462-4192</t>
         </is>
       </c>
     </row>
@@ -979,17 +979,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4442</t>
+          <t>7862</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>6760</t>
+          <t>7551</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4442-6760</t>
+          <t>7862-7551</t>
         </is>
       </c>
     </row>

</xml_diff>